<commit_message>
Update Planilla Control y seguimiento.xlsx
</commit_message>
<xml_diff>
--- a/Planilla Control y seguimiento.xlsx
+++ b/Planilla Control y seguimiento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9a14bdbe45e0146a/Documentos/GitHub/finales/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{E4C6EE95-88FB-4178-A09C-DE4C961E5B61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6DAF8BA4-469B-4A66-B5C4-7CA7C2867468}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{E4C6EE95-88FB-4178-A09C-DE4C961E5B61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{98136DF8-6E01-4294-88C4-FA68DD8C33C3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -384,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -447,23 +447,20 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -471,7 +468,7 @@
   </cellStyles>
   <dxfs count="15">
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -486,7 +483,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1022,7 +1019,7 @@
   <dimension ref="B1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="10" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1036,7 +1033,7 @@
     <col min="7" max="7" width="17" style="17" customWidth="1"/>
     <col min="8" max="8" width="13" style="17" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10" max="11" width="14.33203125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="14.33203125" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1099,13 +1096,13 @@
       <c r="H4" s="18">
         <v>2</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="22">
         <v>43728</v>
       </c>
-      <c r="J4" s="24">
+      <c r="J4" s="5">
         <v>99</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="18">
         <v>11</v>
       </c>
     </row>
@@ -1131,13 +1128,13 @@
       <c r="H5" s="18">
         <v>5</v>
       </c>
-      <c r="I5" s="23">
+      <c r="I5" s="22">
         <v>43728</v>
       </c>
-      <c r="J5" s="24">
+      <c r="J5" s="5">
         <v>99</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="18">
         <v>11</v>
       </c>
     </row>
@@ -1163,13 +1160,13 @@
       <c r="H6" s="18">
         <v>3</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="22">
         <v>43739</v>
       </c>
-      <c r="J6" s="24">
+      <c r="J6" s="5">
         <v>153</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="18">
         <v>17</v>
       </c>
     </row>
@@ -1195,13 +1192,13 @@
       <c r="H7" s="18">
         <v>4</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="22">
         <v>43747</v>
       </c>
-      <c r="J7" s="24">
+      <c r="J7" s="5">
         <v>153</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="18">
         <v>17</v>
       </c>
     </row>
@@ -1227,13 +1224,13 @@
       <c r="H8" s="18">
         <v>1</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="22">
         <v>43752</v>
       </c>
-      <c r="J8" s="24">
+      <c r="J8" s="5">
         <v>243</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="18">
         <v>27</v>
       </c>
     </row>
@@ -1259,13 +1256,13 @@
       <c r="H9" s="18">
         <v>2</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="22">
         <v>43728</v>
       </c>
-      <c r="J9" s="24">
+      <c r="J9" s="5">
         <v>72</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="18">
         <v>8</v>
       </c>
     </row>
@@ -1291,13 +1288,13 @@
       <c r="H10" s="18">
         <v>2</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="22">
         <v>43809</v>
       </c>
-      <c r="J10" s="24">
+      <c r="J10" s="5">
         <v>5</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="18">
         <v>45</v>
       </c>
     </row>
@@ -1323,13 +1320,13 @@
       <c r="H11" s="18">
         <v>75</v>
       </c>
-      <c r="I11" s="23">
+      <c r="I11" s="22">
         <v>43805</v>
       </c>
-      <c r="J11" s="24">
+      <c r="J11" s="5">
         <v>675</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="18">
         <v>75</v>
       </c>
     </row>
@@ -1355,13 +1352,13 @@
       <c r="H12" s="18">
         <v>1</v>
       </c>
-      <c r="I12" s="23">
+      <c r="I12" s="22">
         <v>43762</v>
       </c>
-      <c r="J12" s="24">
+      <c r="J12" s="5">
         <v>140</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="18">
         <v>28</v>
       </c>
     </row>
@@ -1387,11 +1384,11 @@
       <c r="H13" s="18">
         <v>1</v>
       </c>
-      <c r="I13" s="23">
+      <c r="I13" s="22">
         <v>43810</v>
       </c>
-      <c r="J13" s="24"/>
-      <c r="K13" s="4"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="18"/>
     </row>
     <row r="14" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="9" t="s">
@@ -1415,11 +1412,11 @@
       <c r="H14" s="18">
         <v>2</v>
       </c>
-      <c r="I14" s="23">
+      <c r="I14" s="22">
         <v>43810</v>
       </c>
-      <c r="J14" s="24"/>
-      <c r="K14" s="4"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="18"/>
     </row>
     <row r="15" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="9" t="s">
@@ -1443,11 +1440,11 @@
       <c r="H15" s="18">
         <v>5</v>
       </c>
-      <c r="I15" s="23">
+      <c r="I15" s="22">
         <v>43810</v>
       </c>
-      <c r="J15" s="24"/>
-      <c r="K15" s="4"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="18"/>
     </row>
     <row r="16" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="9" t="s">
@@ -1471,9 +1468,11 @@
       <c r="H16" s="18">
         <v>1</v>
       </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="4"/>
+      <c r="I16" s="22">
+        <v>43810</v>
+      </c>
+      <c r="J16" s="5"/>
+      <c r="K16" s="18"/>
     </row>
     <row r="17" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
@@ -1497,13 +1496,13 @@
       <c r="H17" s="18">
         <v>2</v>
       </c>
-      <c r="I17" s="23">
+      <c r="I17" s="22">
         <v>43809</v>
       </c>
-      <c r="J17" s="24">
+      <c r="J17" s="5">
         <v>585</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="18">
         <v>65</v>
       </c>
     </row>
@@ -1520,8 +1519,8 @@
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="4"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="18"/>
     </row>
     <row r="19" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="9" t="s">
@@ -1545,9 +1544,11 @@
       <c r="H19" s="18">
         <v>1</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="4"/>
+      <c r="I19" s="22">
+        <v>43809</v>
+      </c>
+      <c r="J19" s="5"/>
+      <c r="K19" s="18"/>
     </row>
     <row r="20" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
@@ -1571,9 +1572,11 @@
       <c r="H20" s="18">
         <v>1</v>
       </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="4"/>
+      <c r="I20" s="22">
+        <v>43809</v>
+      </c>
+      <c r="J20" s="5"/>
+      <c r="K20" s="18"/>
     </row>
     <row r="21" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="s">
@@ -1597,13 +1600,13 @@
       <c r="H21" s="18">
         <v>3</v>
       </c>
-      <c r="I21" s="23">
+      <c r="I21" s="22">
         <v>43800</v>
       </c>
-      <c r="J21" s="24">
+      <c r="J21" s="5">
         <v>90</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="18">
         <v>10</v>
       </c>
     </row>
@@ -1629,13 +1632,13 @@
       <c r="H22" s="18">
         <v>5</v>
       </c>
-      <c r="I22" s="23">
+      <c r="I22" s="22">
         <v>43803</v>
       </c>
-      <c r="J22" s="24">
+      <c r="J22" s="5">
         <v>99</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K22" s="18">
         <v>11</v>
       </c>
     </row>
@@ -1661,13 +1664,13 @@
       <c r="H23" s="18">
         <v>5</v>
       </c>
-      <c r="I23" s="23">
+      <c r="I23" s="22">
         <v>43803</v>
       </c>
-      <c r="J23" s="24">
+      <c r="J23" s="5">
         <v>99</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="18">
         <v>11</v>
       </c>
     </row>
@@ -1692,8 +1695,8 @@
         <v>1</v>
       </c>
       <c r="I24" s="4"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="4"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="18"/>
     </row>
     <row r="25" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="9" t="s">
@@ -1716,8 +1719,8 @@
         <v>1</v>
       </c>
       <c r="I25" s="4"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="4"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="18"/>
     </row>
     <row r="26" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="9" t="s">
@@ -1741,9 +1744,11 @@
       <c r="H26" s="18">
         <v>1</v>
       </c>
-      <c r="I26" s="4"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="4"/>
+      <c r="I26" s="22">
+        <v>43810</v>
+      </c>
+      <c r="J26" s="5"/>
+      <c r="K26" s="18"/>
     </row>
     <row r="27" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="9" t="s">
@@ -1767,9 +1772,11 @@
       <c r="H27" s="18">
         <v>1</v>
       </c>
-      <c r="I27" s="4"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="4"/>
+      <c r="I27" s="22">
+        <v>43810</v>
+      </c>
+      <c r="J27" s="5"/>
+      <c r="K27" s="18"/>
     </row>
     <row r="28" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="9" t="s">
@@ -1793,9 +1800,11 @@
       <c r="H28" s="18">
         <v>1</v>
       </c>
-      <c r="I28" s="4"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="4"/>
+      <c r="I28" s="22">
+        <v>43810</v>
+      </c>
+      <c r="J28" s="5"/>
+      <c r="K28" s="18"/>
     </row>
     <row r="29" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="9" t="s">
@@ -1819,13 +1828,13 @@
       <c r="H29" s="18">
         <v>1</v>
       </c>
-      <c r="I29" s="23">
+      <c r="I29" s="22">
         <v>43753</v>
       </c>
-      <c r="J29" s="24">
+      <c r="J29" s="5">
         <v>99</v>
       </c>
-      <c r="K29" s="4">
+      <c r="K29" s="18">
         <v>11</v>
       </c>
     </row>
@@ -1851,13 +1860,13 @@
       <c r="H30" s="18">
         <v>7</v>
       </c>
-      <c r="I30" s="23">
+      <c r="I30" s="22">
         <v>43809</v>
       </c>
-      <c r="J30" s="24">
+      <c r="J30" s="5">
         <v>108</v>
       </c>
-      <c r="K30" s="4">
+      <c r="K30" s="18">
         <v>12</v>
       </c>
     </row>
@@ -1883,13 +1892,13 @@
       <c r="H31" s="18">
         <v>5</v>
       </c>
-      <c r="I31" s="23">
+      <c r="I31" s="22">
         <v>43804</v>
       </c>
-      <c r="J31" s="24">
+      <c r="J31" s="5">
         <v>72</v>
       </c>
-      <c r="K31" s="4">
+      <c r="K31" s="18">
         <v>8</v>
       </c>
     </row>
@@ -1915,9 +1924,11 @@
       <c r="H32" s="18">
         <v>5</v>
       </c>
-      <c r="I32" s="4"/>
-      <c r="J32" s="24"/>
-      <c r="K32" s="4"/>
+      <c r="I32" s="22">
+        <v>43810</v>
+      </c>
+      <c r="J32" s="5"/>
+      <c r="K32" s="18"/>
     </row>
     <row r="33" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="9" t="s">
@@ -1941,9 +1952,11 @@
       <c r="H33" s="18">
         <v>5</v>
       </c>
-      <c r="I33" s="4"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="4"/>
+      <c r="I33" s="22">
+        <v>43810</v>
+      </c>
+      <c r="J33" s="5"/>
+      <c r="K33" s="18"/>
     </row>
     <row r="34" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="9" t="s">
@@ -1967,13 +1980,13 @@
       <c r="H34" s="18">
         <v>7</v>
       </c>
-      <c r="I34" s="23">
+      <c r="I34" s="22">
         <v>43755</v>
       </c>
-      <c r="J34" s="24">
+      <c r="J34" s="5">
         <v>63</v>
       </c>
-      <c r="K34" s="4">
+      <c r="K34" s="18">
         <v>7</v>
       </c>
     </row>
@@ -1999,13 +2012,13 @@
       <c r="H35" s="18">
         <v>7</v>
       </c>
-      <c r="I35" s="23">
+      <c r="I35" s="22">
         <v>43800</v>
       </c>
-      <c r="J35" s="24">
+      <c r="J35" s="5">
         <v>351</v>
       </c>
-      <c r="K35" s="4">
+      <c r="K35" s="18">
         <v>39</v>
       </c>
     </row>
@@ -2031,13 +2044,13 @@
       <c r="H36" s="18">
         <v>10</v>
       </c>
-      <c r="I36" s="23">
+      <c r="I36" s="22">
         <v>43801</v>
       </c>
-      <c r="J36" s="24">
+      <c r="J36" s="5">
         <v>306</v>
       </c>
-      <c r="K36" s="4">
+      <c r="K36" s="18">
         <v>34</v>
       </c>
     </row>
@@ -2063,9 +2076,11 @@
       <c r="H37" s="18">
         <v>10</v>
       </c>
-      <c r="I37" s="4"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="4"/>
+      <c r="I37" s="22">
+        <v>43810</v>
+      </c>
+      <c r="J37" s="5"/>
+      <c r="K37" s="18"/>
     </row>
     <row r="38" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="9" t="s">
@@ -2089,13 +2104,13 @@
       <c r="H38" s="18">
         <v>3</v>
       </c>
-      <c r="I38" s="23">
+      <c r="I38" s="22">
         <v>43768</v>
       </c>
-      <c r="J38" s="24">
+      <c r="J38" s="5">
         <v>126</v>
       </c>
-      <c r="K38" s="4">
+      <c r="K38" s="18">
         <v>14</v>
       </c>
     </row>
@@ -2121,11 +2136,11 @@
       <c r="H39" s="18">
         <v>3</v>
       </c>
-      <c r="I39" s="23">
+      <c r="I39" s="22">
         <v>43768</v>
       </c>
-      <c r="J39" s="24"/>
-      <c r="K39" s="4"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="18"/>
     </row>
     <row r="40" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="9" t="s">
@@ -2149,13 +2164,13 @@
       <c r="H40" s="18">
         <v>2</v>
       </c>
-      <c r="I40" s="23">
+      <c r="I40" s="22">
         <v>43808</v>
       </c>
-      <c r="J40" s="24">
+      <c r="J40" s="5">
         <v>153</v>
       </c>
-      <c r="K40" s="4">
+      <c r="K40" s="18">
         <v>17</v>
       </c>
     </row>
@@ -2181,11 +2196,11 @@
       <c r="H41" s="18">
         <v>2</v>
       </c>
-      <c r="I41" s="23">
+      <c r="I41" s="22">
         <v>43810</v>
       </c>
-      <c r="J41" s="24"/>
-      <c r="K41" s="4"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="18"/>
     </row>
     <row r="42" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="9" t="s">
@@ -2209,13 +2224,13 @@
       <c r="H42" s="18">
         <v>5</v>
       </c>
-      <c r="I42" s="23">
+      <c r="I42" s="22">
         <v>43801</v>
       </c>
-      <c r="J42" s="24">
+      <c r="J42" s="5">
         <v>387</v>
       </c>
-      <c r="K42" s="4">
+      <c r="K42" s="18">
         <v>43</v>
       </c>
     </row>
@@ -2241,13 +2256,13 @@
       <c r="H43" s="18">
         <v>5</v>
       </c>
-      <c r="I43" s="27">
+      <c r="I43" s="23">
         <v>43780</v>
       </c>
-      <c r="J43" s="25">
+      <c r="J43" s="24">
         <v>288</v>
       </c>
-      <c r="K43" s="22">
+      <c r="K43" s="26">
         <v>32</v>
       </c>
     </row>
@@ -2273,13 +2288,13 @@
       <c r="H44" s="18">
         <v>5</v>
       </c>
-      <c r="I44" s="23">
+      <c r="I44" s="22">
         <v>43808</v>
       </c>
-      <c r="J44" s="25">
+      <c r="J44" s="24">
         <v>297</v>
       </c>
-      <c r="K44" s="4">
+      <c r="K44" s="18">
         <v>33</v>
       </c>
     </row>
@@ -2305,13 +2320,13 @@
       <c r="H45" s="18">
         <v>5</v>
       </c>
-      <c r="I45" s="27">
+      <c r="I45" s="23">
         <v>43780</v>
       </c>
-      <c r="J45" s="25">
+      <c r="J45" s="24">
         <v>288</v>
       </c>
-      <c r="K45" s="22">
+      <c r="K45" s="26">
         <v>32</v>
       </c>
     </row>
@@ -2337,13 +2352,13 @@
       <c r="H46" s="18">
         <v>5</v>
       </c>
-      <c r="I46" s="23">
+      <c r="I46" s="22">
         <v>43808</v>
       </c>
-      <c r="J46" s="25">
+      <c r="J46" s="24">
         <v>297</v>
       </c>
-      <c r="K46" s="4">
+      <c r="K46" s="18">
         <v>33</v>
       </c>
     </row>
@@ -2369,13 +2384,13 @@
       <c r="H47" s="18">
         <v>5</v>
       </c>
-      <c r="I47" s="27">
+      <c r="I47" s="23">
         <v>43780</v>
       </c>
-      <c r="J47" s="25">
+      <c r="J47" s="24">
         <v>288</v>
       </c>
-      <c r="K47" s="22">
+      <c r="K47" s="26">
         <v>32</v>
       </c>
     </row>
@@ -2401,13 +2416,13 @@
       <c r="H48" s="18">
         <v>5</v>
       </c>
-      <c r="I48" s="23">
+      <c r="I48" s="22">
         <v>43808</v>
       </c>
-      <c r="J48" s="25">
+      <c r="J48" s="24">
         <v>297</v>
       </c>
-      <c r="K48" s="4">
+      <c r="K48" s="18">
         <v>33</v>
       </c>
     </row>
@@ -2432,8 +2447,8 @@
         <v>1</v>
       </c>
       <c r="I49" s="6"/>
-      <c r="J49" s="26"/>
-      <c r="K49" s="6"/>
+      <c r="J49" s="25"/>
+      <c r="K49" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>